<commit_message>
Search in row column matrix.
</commit_message>
<xml_diff>
--- a/DSA(2024).xlsx
+++ b/DSA(2024).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\DSA-2024\DSA(Jan_2024)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\DSA-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418FD9F4-D950-4009-87CE-D6C275903610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF306F5D-76E0-4611-A562-AB2B65E9D31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C961BD99-E443-4C83-B77A-C6824C845070}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -186,6 +186,21 @@
   </si>
   <si>
     <t>Hard</t>
+  </si>
+  <si>
+    <t>On Leave</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Row Column Matrix</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/search-element-sorted-matrix/</t>
+  </si>
+  <si>
+    <t>Search element in a sorted matrix</t>
   </si>
 </sst>
 </file>
@@ -304,6 +319,10 @@
     <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -313,10 +332,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -636,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFF6E4A7-C5AE-40DC-8785-A176246AEA09}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -662,24 +677,24 @@
       <c r="J1" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="15" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="14">
+      <c r="A4" s="16">
         <v>45292</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="17" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -693,8 +708,8 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="7" t="s">
         <v>3</v>
       </c>
@@ -807,10 +822,10 @@
       <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="14">
+      <c r="A13" s="16">
         <v>45299</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="18" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
@@ -824,8 +839,8 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
-      <c r="B14" s="16"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="18"/>
       <c r="C14" t="s">
         <v>22</v>
       </c>
@@ -963,6 +978,86 @@
       </c>
       <c r="E23" s="3" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>45308</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
+        <v>45309</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>45310</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>45311</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="13">
+        <v>45312</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="4">
+        <v>45313</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -989,8 +1084,9 @@
     <hyperlink ref="E19" r:id="rId13" xr:uid="{82CD26CC-A7FA-4082-9C34-D46B59BDE029}"/>
     <hyperlink ref="E22" r:id="rId14" xr:uid="{AA9C4AD2-FDCA-45DD-8530-7E46E675DCF4}"/>
     <hyperlink ref="E23" r:id="rId15" xr:uid="{E4907B01-A708-41EA-A08A-B5F8CB827216}"/>
+    <hyperlink ref="E25" r:id="rId16" xr:uid="{AB61F839-49FF-427B-9942-080E38C4F0A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove Duplicates in-place from Sorted Array.
</commit_message>
<xml_diff>
--- a/DSA(2024).xlsx
+++ b/DSA(2024).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\DSA-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A14CDB-92D1-4E68-96D2-53FD6EA979BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4953989-4F23-4EE5-B3AD-BEA4571AB35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="95">
   <si>
     <t>Task Report DSA(Target 350 Questions with practice-2024)</t>
   </si>
@@ -323,7 +323,13 @@
     <t>https://www.geeksforgeeks.org/problems/check-if-an-array-is-sorted0701/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article</t>
   </si>
   <si>
-    <t>s</t>
+    <t>https://www.geeksforgeeks.org/problems/remove-duplicate-elements-from-sorted-array/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article</t>
+  </si>
+  <si>
+    <t>Find the smallest and second smallest element in an array</t>
+  </si>
+  <si>
+    <t>Remove Duplicates in-place from Sorted Array</t>
   </si>
 </sst>
 </file>
@@ -414,22 +420,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -437,16 +436,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -468,7 +460,31 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -852,62 +868,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41:C42"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.5546875" customWidth="1"/>
     <col min="3" max="3" width="60.88671875" customWidth="1"/>
     <col min="4" max="4" width="16.88671875" customWidth="1"/>
-    <col min="5" max="5" width="107.44140625" customWidth="1"/>
+    <col min="5" max="5" width="107.44140625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F4">
@@ -915,15 +931,15 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="12" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F5">
@@ -931,19 +947,19 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="9" t="s">
         <v>17</v>
       </c>
       <c r="F6">
@@ -951,19 +967,19 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="9" t="s">
         <v>21</v>
       </c>
       <c r="F7">
@@ -971,19 +987,19 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F8">
@@ -991,19 +1007,19 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="9" t="s">
         <v>29</v>
       </c>
       <c r="F9">
@@ -1011,19 +1027,19 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="9" t="s">
         <v>33</v>
       </c>
       <c r="F10">
@@ -1031,26 +1047,26 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="19"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C12" s="12"/>
+      <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
@@ -1059,7 +1075,7 @@
       <c r="D13" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="9" t="s">
         <v>39</v>
       </c>
       <c r="F13">
@@ -1067,8 +1083,8 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="3"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="24"/>
       <c r="C14" t="s">
         <v>40</v>
       </c>
@@ -1077,7 +1093,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B15" t="s">
@@ -1089,7 +1105,7 @@
       <c r="D15" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="9" t="s">
         <v>43</v>
       </c>
       <c r="F15">
@@ -1097,7 +1113,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B16" t="s">
@@ -1109,7 +1125,7 @@
       <c r="D16" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="9" t="s">
         <v>46</v>
       </c>
       <c r="F16">
@@ -1117,19 +1133,19 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B17" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="14" t="s">
         <v>48</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="9" t="s">
         <v>49</v>
       </c>
       <c r="F17">
@@ -1137,7 +1153,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B18" t="s">
@@ -1149,7 +1165,7 @@
       <c r="D18" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="9" t="s">
         <v>52</v>
       </c>
       <c r="F18">
@@ -1157,7 +1173,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B19" t="s">
@@ -1169,7 +1185,7 @@
       <c r="D19" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="9" t="s">
         <v>55</v>
       </c>
       <c r="F19">
@@ -1177,20 +1193,20 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="19"/>
+      <c r="D20" s="13"/>
       <c r="E20" s="19"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B22" t="s">
@@ -1202,7 +1218,7 @@
       <c r="D22" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="9" t="s">
         <v>59</v>
       </c>
       <c r="F22">
@@ -1210,7 +1226,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B23" t="s">
@@ -1222,7 +1238,7 @@
       <c r="D23" t="s">
         <v>62</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="9" t="s">
         <v>63</v>
       </c>
       <c r="F23">
@@ -1230,7 +1246,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B24" t="s">
@@ -1244,7 +1260,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B25" t="s">
@@ -1256,7 +1272,7 @@
       <c r="D25" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="9" t="s">
         <v>68</v>
       </c>
       <c r="F25">
@@ -1264,7 +1280,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B26" t="s">
@@ -1278,7 +1294,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B27" t="s">
@@ -1292,20 +1308,20 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="19"/>
+      <c r="D28" s="13"/>
       <c r="E28" s="19"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B30" t="s">
@@ -1322,7 +1338,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B32" t="s">
@@ -1339,7 +1355,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B33" t="s">
@@ -1356,13 +1372,13 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="C36" s="21"/>
-      <c r="D36" s="22" t="s">
+      <c r="C36" s="15"/>
+      <c r="D36" s="16" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B39" t="s">
@@ -1374,15 +1390,15 @@
       <c r="D39" t="s">
         <v>16</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="14" t="s">
         <v>83</v>
       </c>
       <c r="F39">
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="6" t="s">
+    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B40" t="s">
@@ -1394,7 +1410,7 @@
       <c r="D40" t="s">
         <v>16</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="14" t="s">
         <v>86</v>
       </c>
       <c r="F40">
@@ -1402,19 +1418,19 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" s="20" t="s">
+      <c r="C41" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="14" t="s">
         <v>88</v>
       </c>
       <c r="F41">
@@ -1422,16 +1438,16 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="2"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="20" t="s">
+      <c r="A42" s="25"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="10">
+    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
         <v>45424</v>
       </c>
       <c r="B43" t="s">
@@ -1443,11 +1459,31 @@
       <c r="D43" t="s">
         <v>16</v>
       </c>
-      <c r="E43" s="23" t="s">
+      <c r="E43" s="20" t="s">
         <v>91</v>
       </c>
       <c r="F43">
         <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
+        <v>45425</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F44">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1483,6 +1519,7 @@
     <hyperlink ref="E41" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
     <hyperlink ref="E42" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
     <hyperlink ref="E43" r:id="rId21" xr:uid="{C5CAB132-7B8A-4868-9CE2-EB6967D9E2C5}"/>
+    <hyperlink ref="E44" r:id="rId22" xr:uid="{60C1110F-5F35-4BA3-BE0E-5D2B2A5A0CB4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Left Array roattion kth element.
</commit_message>
<xml_diff>
--- a/DSA(2024).xlsx
+++ b/DSA(2024).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\DSA-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4953989-4F23-4EE5-B3AD-BEA4571AB35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC07E43C-9336-4F6F-88F9-8A6C32117703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="97">
   <si>
     <t>Task Report DSA(Target 350 Questions with practice-2024)</t>
   </si>
@@ -330,6 +330,12 @@
   </si>
   <si>
     <t>Remove Duplicates in-place from Sorted Array</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/problems/rotate-array-by-n-elements-1587115621/1?itm_source=geeksforgeeks&amp;itm_medium=article&amp;itm_campaign=bottom_sticky_on_article</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left Rotate the Array by One And Kth </t>
   </si>
 </sst>
 </file>
@@ -868,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1484,6 +1490,26 @@
       </c>
       <c r="F44">
         <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="3">
+        <v>45427</v>
+      </c>
+      <c r="B45" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" t="s">
+        <v>96</v>
+      </c>
+      <c r="D45" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="F45">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1520,6 +1546,7 @@
     <hyperlink ref="E42" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
     <hyperlink ref="E43" r:id="rId21" xr:uid="{C5CAB132-7B8A-4868-9CE2-EB6967D9E2C5}"/>
     <hyperlink ref="E44" r:id="rId22" xr:uid="{60C1110F-5F35-4BA3-BE0E-5D2B2A5A0CB4}"/>
+    <hyperlink ref="E45" r:id="rId23" xr:uid="{CF0FEC0D-8FF8-4FA8-9FED-790E8E16F911}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Best to Buy and Sell stock
</commit_message>
<xml_diff>
--- a/DSA(2024).xlsx
+++ b/DSA(2024).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\DSA-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23664373-7A56-4186-8158-C7C214462888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B48A92-E3E4-4111-B4B0-35922138A6F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="102">
   <si>
     <t>Task Report DSA(Target 350 Questions with practice-2024)</t>
   </si>
@@ -345,6 +345,12 @@
   </si>
   <si>
     <t>Majority Element (Given an integer array of size n, find all elements that appear more than [n/3] times.</t>
+  </si>
+  <si>
+    <t>Best time to Buy or Sell Stocks.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock/description/</t>
   </si>
 </sst>
 </file>
@@ -441,7 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -493,6 +499,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -506,7 +513,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -890,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -933,10 +940,10 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -953,8 +960,8 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="7" t="s">
         <v>11</v>
       </c>
@@ -1085,10 +1092,10 @@
       <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="25" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
@@ -1105,8 +1112,8 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
-      <c r="B14" s="24"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="25"/>
       <c r="C14" t="s">
         <v>40</v>
       </c>
@@ -1440,16 +1447,16 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="25" t="s">
+      <c r="A41" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="21" t="s">
+      <c r="C41" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="D41" s="21" t="s">
+      <c r="D41" s="22" t="s">
         <v>16</v>
       </c>
       <c r="E41" s="14" t="s">
@@ -1460,10 +1467,10 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="25"/>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
       <c r="E42" s="14" t="s">
         <v>89</v>
       </c>
@@ -1528,12 +1535,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="21" x14ac:dyDescent="0.4">
-      <c r="D49" s="26" t="s">
+    <row r="49" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="D49" s="21" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>45568</v>
       </c>
@@ -1545,6 +1552,23 @@
       </c>
       <c r="D50" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="3">
+        <v>45569</v>
+      </c>
+      <c r="B51" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51" t="s">
+        <v>100</v>
+      </c>
+      <c r="D51" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" s="27" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1582,6 +1606,7 @@
     <hyperlink ref="E43" r:id="rId21" xr:uid="{C5CAB132-7B8A-4868-9CE2-EB6967D9E2C5}"/>
     <hyperlink ref="E44" r:id="rId22" xr:uid="{60C1110F-5F35-4BA3-BE0E-5D2B2A5A0CB4}"/>
     <hyperlink ref="E45" r:id="rId23" xr:uid="{CF0FEC0D-8FF8-4FA8-9FED-790E8E16F911}"/>
+    <hyperlink ref="E51" r:id="rId24" xr:uid="{9DAD39F5-2A80-4390-9BA5-B159E91EB2B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Find the missing number
</commit_message>
<xml_diff>
--- a/DSA(2024).xlsx
+++ b/DSA(2024).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\DSA-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76266835-A40F-4D82-81B7-CAD164A51660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022A8738-C898-430F-B840-603F0A813061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="104">
   <si>
     <t>Task Report DSA(Target 350 Questions with practice-2024)</t>
   </si>
@@ -355,6 +355,9 @@
   <si>
     <t>Find valid anagram</t>
   </si>
+  <si>
+    <t>Find the missing number [1 to N]</t>
+  </si>
 </sst>
 </file>
 
@@ -364,7 +367,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="165" formatCode="mm/yy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -422,6 +425,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -450,7 +459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -516,6 +525,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -900,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1045,7 +1060,7 @@
       <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="28" t="s">
         <v>28</v>
       </c>
       <c r="D9" t="s">
@@ -1505,7 +1520,7 @@
       <c r="B44" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C44" s="29" t="s">
         <v>94</v>
       </c>
       <c r="D44" t="s">
@@ -1585,6 +1600,20 @@
         <v>102</v>
       </c>
       <c r="D52" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="3">
+        <v>45607</v>
+      </c>
+      <c r="B53" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" t="s">
+        <v>103</v>
+      </c>
+      <c r="D53" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>